<commit_message>
add more exploration of variables
</commit_message>
<xml_diff>
--- a/data/lit/lit_summary-penalty-over-years.xlsx
+++ b/data/lit/lit_summary-penalty-over-years.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gina Laptippytop\Documents\_git_repos\ghproj_ccgap\_data\lit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gina Laptippytop\Documents\_git_repos\ghproj_ccgap\data\lit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B69C8C64-2756-4ABB-B203-E691965F2824}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8213C683-C13C-406F-9C40-EE9FC08986EB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{F284945C-B536-4792-BD89-54D1A7087DE1}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="64">
   <si>
     <t>years_in_corn</t>
   </si>
@@ -74,9 +74,6 @@
     <t>notes2</t>
   </si>
   <si>
-    <t>reason given is residue</t>
-  </si>
-  <si>
     <t>Crookston et al. 1991</t>
   </si>
   <si>
@@ -195,6 +192,39 @@
   </si>
   <si>
     <t>tillage</t>
+  </si>
+  <si>
+    <t>moldboard fall, spring disk</t>
+  </si>
+  <si>
+    <t>n_mgmt</t>
+  </si>
+  <si>
+    <t>aonr</t>
+  </si>
+  <si>
+    <t>chisel-plow fall, cultivated spring</t>
+  </si>
+  <si>
+    <t>year is confounded with #years in corn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yield gap determined from regression equations at AONR, not actually measured. </t>
+  </si>
+  <si>
+    <t>Used different N rates each year</t>
+  </si>
+  <si>
+    <t>7th year corn received smallest N rate</t>
+  </si>
+  <si>
+    <t>varies</t>
+  </si>
+  <si>
+    <t>farmer choice</t>
+  </si>
+  <si>
+    <t>multiple rates</t>
   </si>
 </sst>
 </file>
@@ -665,18 +695,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -727,7 +757,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -778,7 +808,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -829,7 +859,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -885,19 +915,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3571DFEC-2EAC-47F6-AAE2-490ED5BF3FEC}">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="31" customWidth="1"/>
-    <col min="4" max="5" width="32.44140625" customWidth="1"/>
+    <col min="4" max="6" width="32.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -911,16 +941,19 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -933,8 +966,14 @@
       <c r="D2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -944,8 +983,14 @@
       <c r="C3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -955,8 +1000,14 @@
       <c r="C4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -966,8 +1017,14 @@
       <c r="C5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -977,8 +1034,14 @@
       <c r="C6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -991,11 +1054,17 @@
       <c r="D7" t="s">
         <v>7</v>
       </c>
-      <c r="G7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>3</v>
       </c>
@@ -1005,11 +1074,20 @@
       <c r="C8" t="s">
         <v>6</v>
       </c>
+      <c r="E8" t="s">
+        <v>56</v>
+      </c>
       <c r="F8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>5</v>
       </c>
@@ -1019,11 +1097,20 @@
       <c r="C9" t="s">
         <v>6</v>
       </c>
+      <c r="E9" t="s">
+        <v>56</v>
+      </c>
       <c r="F9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>7</v>
       </c>
@@ -1033,11 +1120,20 @@
       <c r="C10" t="s">
         <v>6</v>
       </c>
+      <c r="E10" t="s">
+        <v>56</v>
+      </c>
       <c r="F10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1045,13 +1141,19 @@
         <v>100</v>
       </c>
       <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
         <v>14</v>
       </c>
-      <c r="D11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2</v>
       </c>
@@ -1059,10 +1161,16 @@
         <v>84.615384615384599</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+      <c r="E12" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>3</v>
       </c>
@@ -1070,10 +1178,16 @@
         <v>87.912087912087898</v>
       </c>
       <c r="C13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+      <c r="E13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>4</v>
       </c>
@@ -1081,10 +1195,16 @@
         <v>87.912087912087898</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+      <c r="E14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>5</v>
       </c>
@@ -1092,10 +1212,16 @@
         <v>86.813186813186803</v>
       </c>
       <c r="C15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+      <c r="E15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1103,13 +1229,19 @@
         <v>100</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="E16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1117,10 +1249,16 @@
         <v>88.794153471376305</v>
       </c>
       <c r="C17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="E17" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>3</v>
       </c>
@@ -1128,10 +1266,16 @@
         <v>89.646772228988993</v>
       </c>
       <c r="C18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="E18" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>4</v>
       </c>
@@ -1139,10 +1283,16 @@
         <v>89.524969549329995</v>
       </c>
       <c r="C19" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="E19" t="s">
+        <v>53</v>
+      </c>
+      <c r="F19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>5</v>
       </c>
@@ -1150,10 +1300,16 @@
         <v>86.601705237515205</v>
       </c>
       <c r="C20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="E20" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>10</v>
       </c>
@@ -1161,10 +1317,16 @@
         <v>88.185140073081598</v>
       </c>
       <c r="C21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="E21" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1172,13 +1334,19 @@
         <v>100</v>
       </c>
       <c r="C22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="E22" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1186,10 +1354,16 @@
         <v>89.696312364425097</v>
       </c>
       <c r="C23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="E23" t="s">
+        <v>53</v>
+      </c>
+      <c r="F23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>3</v>
       </c>
@@ -1197,10 +1371,16 @@
         <v>88.069414316702805</v>
       </c>
       <c r="C24" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="E24" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>4</v>
       </c>
@@ -1208,10 +1388,16 @@
         <v>88.720173535791702</v>
       </c>
       <c r="C25" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="E25" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>5</v>
       </c>
@@ -1219,10 +1405,16 @@
         <v>90.347071583514094</v>
       </c>
       <c r="C26" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="E26" t="s">
+        <v>53</v>
+      </c>
+      <c r="F26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>10</v>
       </c>
@@ -1230,10 +1422,16 @@
         <v>88.177874186550895</v>
       </c>
       <c r="C27" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="E27" t="s">
+        <v>53</v>
+      </c>
+      <c r="F27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1241,13 +1439,19 @@
         <v>100</v>
       </c>
       <c r="C28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D28" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+      <c r="E28" t="s">
+        <v>53</v>
+      </c>
+      <c r="F28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2</v>
       </c>
@@ -1255,10 +1459,16 @@
         <v>89.414182939362703</v>
       </c>
       <c r="C29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="E29" t="s">
+        <v>53</v>
+      </c>
+      <c r="F29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>3</v>
       </c>
@@ -1266,10 +1476,16 @@
         <v>85.611510791366896</v>
       </c>
       <c r="C30" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="E30" t="s">
+        <v>53</v>
+      </c>
+      <c r="F30" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>4</v>
       </c>
@@ -1277,10 +1493,16 @@
         <v>85.303186022610404</v>
       </c>
       <c r="C31" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="E31" t="s">
+        <v>53</v>
+      </c>
+      <c r="F31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>5</v>
       </c>
@@ -1288,10 +1510,16 @@
         <v>86.022610483042101</v>
       </c>
       <c r="C32" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="E32" t="s">
+        <v>53</v>
+      </c>
+      <c r="F32" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>10</v>
       </c>
@@ -1299,10 +1527,16 @@
         <v>84.275436793422401</v>
       </c>
       <c r="C33" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="E33" t="s">
+        <v>53</v>
+      </c>
+      <c r="F33" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>1</v>
       </c>
@@ -1310,13 +1544,19 @@
         <v>100</v>
       </c>
       <c r="C34" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" t="s">
         <v>17</v>
       </c>
-      <c r="D34" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E34" t="s">
+        <v>53</v>
+      </c>
+      <c r="F34" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>2</v>
       </c>
@@ -1324,10 +1564,16 @@
         <v>85</v>
       </c>
       <c r="C35" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="E35" t="s">
+        <v>53</v>
+      </c>
+      <c r="F35" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>3</v>
       </c>
@@ -1335,7 +1581,13 @@
         <v>85</v>
       </c>
       <c r="C36" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="E36" t="s">
+        <v>53</v>
+      </c>
+      <c r="F36" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1367,22 +1619,22 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" t="s">
-        <v>27</v>
-      </c>
       <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
         <v>32</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>33</v>
-      </c>
-      <c r="G1" t="s">
-        <v>34</v>
       </c>
       <c r="H1" t="s">
         <v>8</v>
@@ -1390,15 +1642,15 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -1410,7 +1662,7 @@
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="E3" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
@@ -1422,10 +1674,10 @@
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>30</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>31</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="8"/>
@@ -1436,10 +1688,10 @@
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="8"/>
@@ -1452,7 +1704,7 @@
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H6" s="8"/>
     </row>
@@ -1462,10 +1714,10 @@
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="8"/>
@@ -1476,47 +1728,47 @@
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="10" t="s">
-        <v>38</v>
-      </c>
       <c r="G8" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H8" s="12"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" t="s">
         <v>42</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" t="s">
-        <v>46</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H9" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>